<commit_message>
Updated some of the column titles in results/data
</commit_message>
<xml_diff>
--- a/AnimalShelterPoster - Data.xlsx
+++ b/AnimalShelterPoster - Data.xlsx
@@ -52,13 +52,13 @@
     <t>Number of Animals Training</t>
   </si>
   <si>
-    <t>Training Set</t>
+    <t>Percent of Training Set with Outcome</t>
   </si>
   <si>
     <t>Number of Animals Testing</t>
   </si>
   <si>
-    <t>Testing Set</t>
+    <t>Percent of Testing Set with Outcome</t>
   </si>
   <si>
     <t>intactness</t>
@@ -256,11 +256,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1538655678"/>
-        <c:axId val="1117649543"/>
+        <c:axId val="1892907292"/>
+        <c:axId val="81905116"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1538655678"/>
+        <c:axId val="1892907292"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -302,10 +302,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1117649543"/>
+        <c:crossAx val="81905116"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1117649543"/>
+        <c:axId val="81905116"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -363,7 +363,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1538655678"/>
+        <c:crossAx val="1892907292"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -464,11 +464,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="89214524"/>
-        <c:axId val="505128945"/>
+        <c:axId val="977376684"/>
+        <c:axId val="896108397"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="89214524"/>
+        <c:axId val="977376684"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -510,10 +510,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="505128945"/>
+        <c:crossAx val="896108397"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="505128945"/>
+        <c:axId val="896108397"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -571,7 +571,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89214524"/>
+        <c:crossAx val="977376684"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -695,11 +695,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1292347592"/>
-        <c:axId val="555060312"/>
+        <c:axId val="1098532226"/>
+        <c:axId val="601114164"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1292347592"/>
+        <c:axId val="1098532226"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -741,10 +741,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="555060312"/>
+        <c:crossAx val="601114164"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="555060312"/>
+        <c:axId val="601114164"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -802,7 +802,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1292347592"/>
+        <c:crossAx val="1098532226"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -894,11 +894,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="359101924"/>
-        <c:axId val="200818932"/>
+        <c:axId val="1786318213"/>
+        <c:axId val="689606281"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="359101924"/>
+        <c:axId val="1786318213"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -940,10 +940,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="200818932"/>
+        <c:crossAx val="689606281"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200818932"/>
+        <c:axId val="689606281"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1001,7 +1001,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359101924"/>
+        <c:crossAx val="1786318213"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1086,11 +1086,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1043238985"/>
-        <c:axId val="1356038652"/>
+        <c:axId val="107969468"/>
+        <c:axId val="413201110"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1043238985"/>
+        <c:axId val="107969468"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1132,10 +1132,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1356038652"/>
+        <c:crossAx val="413201110"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1356038652"/>
+        <c:axId val="413201110"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1193,7 +1193,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1043238985"/>
+        <c:crossAx val="107969468"/>
       </c:valAx>
     </c:plotArea>
   </c:chart>
@@ -1259,11 +1259,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2113482803"/>
-        <c:axId val="430332035"/>
+        <c:axId val="851951868"/>
+        <c:axId val="579843674"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2113482803"/>
+        <c:axId val="851951868"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1305,10 +1305,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="430332035"/>
+        <c:crossAx val="579843674"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="430332035"/>
+        <c:axId val="579843674"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1366,7 +1366,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2113482803"/>
+        <c:crossAx val="851951868"/>
       </c:valAx>
     </c:plotArea>
   </c:chart>

</xml_diff>